<commit_message>
added functions to mimic data.csv
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -20,23 +20,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t xml:space="preserve">b</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">←</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="[$-409]MM/DD/YY"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -103,8 +112,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -125,34 +146,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>2</v>
-      </c>
+      <c r="A1" s="1" t="n">
+        <v>34262</v>
+      </c>
+      <c r="B1" s="2"/>
       <c r="C1" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>43761</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the multi read-xlsx to work on both low level and high level
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -41,11 +41,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="[$-409]MM/DD/YY"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -112,20 +110,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,7 +139,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -161,7 +151,6 @@
       <c r="A1" s="1" t="n">
         <v>34262</v>
       </c>
-      <c r="B1" s="2"/>
       <c r="C1" s="0" t="n">
         <v>3</v>
       </c>
@@ -186,7 +175,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="1" t="n">
         <f aca="true">TODAY()</f>
         <v>43761</v>
       </c>

</xml_diff>

<commit_message>
added functions on both low and high level to list all sheets on a xlsx file, incremented the project version, added examples
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -5,10 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Second Sheet" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Third Sheet" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Last Sheet" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -138,7 +141,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -177,7 +180,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>43761</v>
+        <v>43766</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>4</v>
@@ -192,4 +195,82 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>